<commit_message>
last update project product search
search google shopping and bucape
</commit_message>
<xml_diff>
--- a/35 - Automação Web - Aplicação de Mercado ao Trabalho/Projeto 2 - Google Shopping e Buscape/buscas.xlsx
+++ b/35 - Automação Web - Aplicação de Mercado ao Trabalho/Projeto 2 - Google Shopping e Buscape/buscas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thiarly/Library/CloudStorage/GoogleDrive-thiarly.cavalcante@gmail.com/My Drive/PROJECTS/Impressionador-Python-Course/35 - Automação Web - Aplicação de Mercado ao Trabalho/Projeto 2 - Google Shopping e Buscape/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0F9637-B4A8-7242-842E-1677783457FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EA2EDB-A42A-2644-8143-98B370042A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="13160" xr2:uid="{CD3F9E8B-8E7C-43BA-8194-A874F6873E6D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Nome</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>iphone 12 64 gb</t>
+  </si>
+  <si>
+    <t>keychron k3 pro</t>
+  </si>
+  <si>
+    <t>v2</t>
   </si>
 </sst>
 </file>
@@ -418,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220DEAF8-BE44-4105-B361-44B3C8893CB3}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -454,10 +460,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>3000</v>
+        <v>2500</v>
       </c>
       <c r="D2">
-        <v>3500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -468,10 +474,24 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="D3">
-        <v>4500</v>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+      <c r="D4">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update busca google e buscape
</commit_message>
<xml_diff>
--- a/35 - Automação Web - Aplicação de Mercado ao Trabalho/Projeto 2 - Google Shopping e Buscape/buscas.xlsx
+++ b/35 - Automação Web - Aplicação de Mercado ao Trabalho/Projeto 2 - Google Shopping e Buscape/buscas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thiarly/Library/CloudStorage/GoogleDrive-thiarly.cavalcante@gmail.com/My Drive/PROJECTS/Impressionador-Python-Course/35 - Automação Web - Aplicação de Mercado ao Trabalho/Projeto 2 - Google Shopping e Buscape/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thiarly/Library/CloudStorage/GoogleDrive-thiarly.cavalcante@gmail.com/My Drive/PROJECTS/Impressionador-Python-Course/35 - Automação Web - Aplicação de Mercado ao Trabalho/Projeto 2 - Google Shopping e Buscape/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EA2EDB-A42A-2644-8143-98B370042A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1D35AD-B9DD-B145-BCF2-A4F045349BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="13160" xr2:uid="{CD3F9E8B-8E7C-43BA-8194-A874F6873E6D}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -460,10 +460,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="D2">
-        <v>5000</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -477,7 +477,7 @@
         <v>2000</v>
       </c>
       <c r="D3">
-        <v>5000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>